<commit_message>
Final commit to enusre everyting has been updated
</commit_message>
<xml_diff>
--- a/Main_Assignment/p.xlsx
+++ b/Main_Assignment/p.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2420" yWindow="2420" windowWidth="14400" windowHeight="7360" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name=" Sheet 2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -643,7 +643,7 @@
           <t>abc</t>
         </is>
       </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>abc</t>
         </is>
@@ -657,6 +657,29 @@
         <v>8861772198</v>
       </c>
       <c r="E9" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>pr</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>qeh@gmail.com</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>884692</v>
+      </c>
+      <c r="E10" t="n">
         <v>23</v>
       </c>
     </row>
@@ -678,7 +701,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>

</xml_diff>